<commit_message>
New data and Update
</commit_message>
<xml_diff>
--- a/Phenoloxidase Activity data/82. HEG 32 (91214).xlsx
+++ b/Phenoloxidase Activity data/82. HEG 32 (91214).xlsx
@@ -64,34 +64,34 @@
     <t>Sample 91153</t>
   </si>
   <si>
-    <t>F1</t>
+    <t>C1</t>
   </si>
   <si>
-    <t>F2</t>
+    <t>C2</t>
   </si>
   <si>
-    <t>F3</t>
+    <t>C3</t>
   </si>
   <si>
-    <t>F4</t>
+    <t>C4</t>
   </si>
   <si>
-    <t>F5</t>
+    <t>C5</t>
   </si>
   <si>
-    <t>F6</t>
+    <t>C6</t>
   </si>
   <si>
-    <t>H10</t>
+    <t>G1</t>
   </si>
   <si>
-    <t>H11</t>
+    <t>G2</t>
   </si>
   <si>
-    <t>H12</t>
+    <t>G3</t>
   </si>
   <si>
-    <t>HEG - 31</t>
+    <t>HEG - 32</t>
   </si>
 </sst>
 </file>
@@ -369,37 +369,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.3289999961853027</c:v>
+                  <c:v>0.8880000114440918</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3059999942779541</c:v>
+                  <c:v>0.8848000168800354</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2795000076293945</c:v>
+                  <c:v>0.87720000743865967</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2847000360488892</c:v>
+                  <c:v>0.87529999017715454</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2824000120162964</c:v>
+                  <c:v>0.87760001420974731</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2856999635696411</c:v>
+                  <c:v>0.87650001049041748</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2853000164031982</c:v>
+                  <c:v>0.87589997053146362</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.2868000268936157</c:v>
+                  <c:v>0.87459999322891235</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.2869999408721924</c:v>
+                  <c:v>0.87319999933242798</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.2861000299453735</c:v>
+                  <c:v>0.87339997291564941</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.2847000360488892</c:v>
+                  <c:v>0.87290000915527344</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -414,11 +414,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="237665768"/>
-        <c:axId val="237668512"/>
+        <c:axId val="300954520"/>
+        <c:axId val="300951776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="237665768"/>
+        <c:axId val="300954520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -475,12 +475,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237668512"/>
+        <c:crossAx val="300951776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="237668512"/>
+        <c:axId val="300951776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -537,7 +537,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237665768"/>
+        <c:crossAx val="300954520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -761,37 +761,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.399399995803833</c:v>
+                  <c:v>0.86239999532699585</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3833999633789063</c:v>
+                  <c:v>0.857200026512146</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3614000082015991</c:v>
+                  <c:v>0.84170001745223999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3514000177383423</c:v>
+                  <c:v>0.84530001878738403</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3507000207901001</c:v>
+                  <c:v>0.84049999713897705</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.351099967956543</c:v>
+                  <c:v>0.83960002660751343</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3523999452590942</c:v>
+                  <c:v>0.83850002288818359</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3540999889373779</c:v>
+                  <c:v>0.83600002527236938</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3549000024795532</c:v>
+                  <c:v>0.83520001173019409</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.3532999753952026</c:v>
+                  <c:v>0.83410000801086426</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.3529000282287598</c:v>
+                  <c:v>0.8345000147819519</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -806,11 +806,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="237666552"/>
-        <c:axId val="237666944"/>
+        <c:axId val="300950208"/>
+        <c:axId val="300950600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="237666552"/>
+        <c:axId val="300950208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -867,12 +867,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237666944"/>
+        <c:crossAx val="300950600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="237666944"/>
+        <c:axId val="300950600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -929,7 +929,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="237666552"/>
+        <c:crossAx val="300950208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1153,37 +1153,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.3622000217437744</c:v>
+                  <c:v>0.90740001201629639</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3263000249862671</c:v>
+                  <c:v>0.89139997959136963</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3035999536514282</c:v>
+                  <c:v>0.88730001449584961</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.312999963760376</c:v>
+                  <c:v>0.88489997386932373</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.3071000576019287</c:v>
+                  <c:v>0.88510000705718994</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.3101999759674072</c:v>
+                  <c:v>0.88580000400543213</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3055000305175781</c:v>
+                  <c:v>0.88550001382827759</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3092000484466553</c:v>
+                  <c:v>0.88569998741149902</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3027000427246094</c:v>
+                  <c:v>0.88539999723434448</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.304900050163269</c:v>
+                  <c:v>0.88529998064041138</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.305899977684021</c:v>
+                  <c:v>0.88499999046325684</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1198,11 +1198,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="239750264"/>
-        <c:axId val="239753008"/>
+        <c:axId val="300951384"/>
+        <c:axId val="300953344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="239750264"/>
+        <c:axId val="300951384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1259,12 +1259,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239753008"/>
+        <c:crossAx val="300953344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="239753008"/>
+        <c:axId val="300953344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1321,7 +1321,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239750264"/>
+        <c:crossAx val="300951384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1545,37 +1545,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.3969000577926636</c:v>
+                  <c:v>0.74210000038146973</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4208999872207642</c:v>
+                  <c:v>0.75840002298355103</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4388999938964844</c:v>
+                  <c:v>0.77259999513626099</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4895999431610107</c:v>
+                  <c:v>0.7882000207901001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5183999538421631</c:v>
+                  <c:v>0.79540002346038818</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5471999645233154</c:v>
+                  <c:v>0.81190001964569092</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5745999813079834</c:v>
+                  <c:v>0.82440000772476196</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.6004999876022339</c:v>
+                  <c:v>0.8343999981880188</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.6236000061035156</c:v>
+                  <c:v>0.84450000524520874</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.6440999507904053</c:v>
+                  <c:v>0.85280001163482666</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.6655000448226929</c:v>
+                  <c:v>0.86330002546310425</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1590,11 +1590,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="239752224"/>
-        <c:axId val="239755752"/>
+        <c:axId val="300953736"/>
+        <c:axId val="300954912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="239752224"/>
+        <c:axId val="300953736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1651,12 +1651,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239755752"/>
+        <c:crossAx val="300954912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="239755752"/>
+        <c:axId val="300954912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1713,7 +1713,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239752224"/>
+        <c:crossAx val="300953736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1937,37 +1937,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.3562999963760376</c:v>
+                  <c:v>0.82499998807907104</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3845000267028809</c:v>
+                  <c:v>0.82160001993179321</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4154000282287598</c:v>
+                  <c:v>0.80909997224807739</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4664000272750854</c:v>
+                  <c:v>0.8180999755859375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4980000257492065</c:v>
+                  <c:v>0.83279997110366821</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5290999412536621</c:v>
+                  <c:v>0.83939999341964722</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5597000122070313</c:v>
+                  <c:v>0.8475000262260437</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.5860999822616577</c:v>
+                  <c:v>0.86009997129440308</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.6126999855041504</c:v>
+                  <c:v>0.87599998712539673</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.6338000297546387</c:v>
+                  <c:v>0.88910001516342163</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.6562999486923218</c:v>
+                  <c:v>0.90630000829696655</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1982,11 +1982,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="239756928"/>
-        <c:axId val="239756144"/>
+        <c:axId val="243791480"/>
+        <c:axId val="243791872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="239756928"/>
+        <c:axId val="243791480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2043,12 +2043,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239756144"/>
+        <c:crossAx val="243791872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="239756144"/>
+        <c:axId val="243791872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2105,7 +2105,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239756928"/>
+        <c:crossAx val="243791480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2329,37 +2329,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.4602999687194824</c:v>
+                  <c:v>0.99059998989105225</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4881000518798828</c:v>
+                  <c:v>0.99639999866485596</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5125000476837158</c:v>
+                  <c:v>1.006100058555603</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5582000017166138</c:v>
+                  <c:v>1.0099999904632568</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5859999656677246</c:v>
+                  <c:v>1.0205999612808228</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6171000003814697</c:v>
+                  <c:v>1.0288000106811523</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6435999870300293</c:v>
+                  <c:v>1.0318000316619873</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.6694999933242798</c:v>
+                  <c:v>1.0420999526977539</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.6948000192642212</c:v>
+                  <c:v>1.0469000339508057</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.7158999443054199</c:v>
+                  <c:v>1.0493999719619751</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.7395999431610107</c:v>
+                  <c:v>1.0592999458312988</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2374,11 +2374,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="239757320"/>
-        <c:axId val="239754184"/>
+        <c:axId val="243791088"/>
+        <c:axId val="243788344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="239757320"/>
+        <c:axId val="243791088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2435,12 +2435,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239754184"/>
+        <c:crossAx val="243788344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="239754184"/>
+        <c:axId val="243788344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2497,7 +2497,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239757320"/>
+        <c:crossAx val="243791088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2721,37 +2721,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.468999981880188</c:v>
+                  <c:v>0.8726000189781189</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5075000524520874</c:v>
+                  <c:v>0.89840000867843628</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5296000242233276</c:v>
+                  <c:v>0.90429997444152832</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5700000524520874</c:v>
+                  <c:v>0.91540002822875977</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5918999910354614</c:v>
+                  <c:v>0.92510002851486206</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6202000379562378</c:v>
+                  <c:v>0.93819999694824219</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6440999507904053</c:v>
+                  <c:v>0.94849997758865356</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.6651999950408936</c:v>
+                  <c:v>0.96079999208450317</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.687999963760376</c:v>
+                  <c:v>0.97310000658035278</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.7039999961853027</c:v>
+                  <c:v>0.98290002346038818</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.7206000089645386</c:v>
+                  <c:v>0.99459999799728394</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2766,11 +2766,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="239751440"/>
-        <c:axId val="239751832"/>
+        <c:axId val="299736680"/>
+        <c:axId val="388541176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="239751440"/>
+        <c:axId val="299736680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2827,12 +2827,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239751832"/>
+        <c:crossAx val="388541176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="239751832"/>
+        <c:axId val="388541176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2889,7 +2889,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="239751440"/>
+        <c:crossAx val="299736680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3113,37 +3113,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.4392999410629272</c:v>
+                  <c:v>0.79860001802444458</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4795000553131104</c:v>
+                  <c:v>0.80739998817443848</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5166000127792358</c:v>
+                  <c:v>0.81650000810623169</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5621999502182007</c:v>
+                  <c:v>0.82719999551773071</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5843000411987305</c:v>
+                  <c:v>0.83890002965927124</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6066000461578369</c:v>
+                  <c:v>0.84939998388290405</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6277999877929687</c:v>
+                  <c:v>0.86009997129440308</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.6492999792098999</c:v>
+                  <c:v>0.87070000171661377</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.6711000204086304</c:v>
+                  <c:v>0.88129997253417969</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.6893999576568604</c:v>
+                  <c:v>0.89179998636245728</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.7085000276565552</c:v>
+                  <c:v>0.90179997682571411</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3158,11 +3158,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="240385768"/>
-        <c:axId val="240384984"/>
+        <c:axId val="388538824"/>
+        <c:axId val="388540784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="240385768"/>
+        <c:axId val="388538824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3219,12 +3219,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240384984"/>
+        <c:crossAx val="388540784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="240384984"/>
+        <c:axId val="388540784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3281,7 +3281,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240385768"/>
+        <c:crossAx val="388538824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3505,37 +3505,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>1.4384000301361084</c:v>
+                  <c:v>0.86070001125335693</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4737000465393066</c:v>
+                  <c:v>0.8694000244140625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4991999864578247</c:v>
+                  <c:v>0.87449997663497925</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5490000247955322</c:v>
+                  <c:v>0.88440001010894775</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5776000022888184</c:v>
+                  <c:v>0.90039998292922974</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6019999980926514</c:v>
+                  <c:v>0.91720002889633179</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6211999654769897</c:v>
+                  <c:v>0.93580001592636108</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.638200044631958</c:v>
+                  <c:v>0.95469999313354492</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.6539000272750854</c:v>
+                  <c:v>0.9725000262260437</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.6684000492095947</c:v>
+                  <c:v>0.99029999971389771</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.68340003490448</c:v>
+                  <c:v>1.0054999589920044</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3550,11 +3550,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="240389296"/>
-        <c:axId val="240391256"/>
+        <c:axId val="388539216"/>
+        <c:axId val="388534120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="240389296"/>
+        <c:axId val="388539216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3611,12 +3611,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240391256"/>
+        <c:crossAx val="388534120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="240391256"/>
+        <c:axId val="388534120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3673,7 +3673,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="240389296"/>
+        <c:crossAx val="388539216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9289,7 +9289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:L3"/>
     </sheetView>
   </sheetViews>
@@ -9303,37 +9303,37 @@
         <v>18</v>
       </c>
       <c r="B1" s="1">
-        <v>1.3289999961853027</v>
+        <v>0.8880000114440918</v>
       </c>
       <c r="C1" s="1">
-        <v>1.3059999942779541</v>
+        <v>0.8848000168800354</v>
       </c>
       <c r="D1" s="1">
-        <v>1.2795000076293945</v>
+        <v>0.87720000743865967</v>
       </c>
       <c r="E1" s="1">
-        <v>1.2847000360488892</v>
+        <v>0.87529999017715454</v>
       </c>
       <c r="F1" s="1">
-        <v>1.2824000120162964</v>
+        <v>0.87760001420974731</v>
       </c>
       <c r="G1" s="1">
-        <v>1.2856999635696411</v>
+        <v>0.87650001049041748</v>
       </c>
       <c r="H1" s="1">
-        <v>1.2853000164031982</v>
+        <v>0.87589997053146362</v>
       </c>
       <c r="I1" s="1">
-        <v>1.2868000268936157</v>
+        <v>0.87459999322891235</v>
       </c>
       <c r="J1" s="1">
-        <v>1.2869999408721924</v>
+        <v>0.87319999933242798</v>
       </c>
       <c r="K1" s="1">
-        <v>1.2861000299453735</v>
+        <v>0.87339997291564941</v>
       </c>
       <c r="L1" s="1">
-        <v>1.2847000360488892</v>
+        <v>0.87290000915527344</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
@@ -9341,37 +9341,37 @@
         <v>19</v>
       </c>
       <c r="B2" s="1">
-        <v>1.399399995803833</v>
+        <v>0.86239999532699585</v>
       </c>
       <c r="C2" s="1">
-        <v>1.3833999633789063</v>
+        <v>0.857200026512146</v>
       </c>
       <c r="D2" s="1">
-        <v>1.3614000082015991</v>
+        <v>0.84170001745223999</v>
       </c>
       <c r="E2" s="1">
-        <v>1.3514000177383423</v>
+        <v>0.84530001878738403</v>
       </c>
       <c r="F2" s="1">
-        <v>1.3507000207901001</v>
+        <v>0.84049999713897705</v>
       </c>
       <c r="G2" s="1">
-        <v>1.351099967956543</v>
+        <v>0.83960002660751343</v>
       </c>
       <c r="H2" s="1">
-        <v>1.3523999452590942</v>
+        <v>0.83850002288818359</v>
       </c>
       <c r="I2" s="1">
-        <v>1.3540999889373779</v>
+        <v>0.83600002527236938</v>
       </c>
       <c r="J2" s="1">
-        <v>1.3549000024795532</v>
+        <v>0.83520001173019409</v>
       </c>
       <c r="K2" s="1">
-        <v>1.3532999753952026</v>
+        <v>0.83410000801086426</v>
       </c>
       <c r="L2" s="1">
-        <v>1.3529000282287598</v>
+        <v>0.8345000147819519</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
@@ -9379,37 +9379,37 @@
         <v>20</v>
       </c>
       <c r="B3" s="1">
-        <v>1.3622000217437744</v>
+        <v>0.90740001201629639</v>
       </c>
       <c r="C3" s="1">
-        <v>1.3263000249862671</v>
+        <v>0.89139997959136963</v>
       </c>
       <c r="D3" s="1">
-        <v>1.3035999536514282</v>
+        <v>0.88730001449584961</v>
       </c>
       <c r="E3" s="1">
-        <v>1.312999963760376</v>
+        <v>0.88489997386932373</v>
       </c>
       <c r="F3" s="1">
-        <v>1.3071000576019287</v>
+        <v>0.88510000705718994</v>
       </c>
       <c r="G3" s="1">
-        <v>1.3101999759674072</v>
+        <v>0.88580000400543213</v>
       </c>
       <c r="H3" s="1">
-        <v>1.3055000305175781</v>
+        <v>0.88550001382827759</v>
       </c>
       <c r="I3" s="1">
-        <v>1.3092000484466553</v>
+        <v>0.88569998741149902</v>
       </c>
       <c r="J3" s="1">
-        <v>1.3027000427246094</v>
+        <v>0.88539999723434448</v>
       </c>
       <c r="K3" s="1">
-        <v>1.304900050163269</v>
+        <v>0.88529998064041138</v>
       </c>
       <c r="L3" s="1">
-        <v>1.305899977684021</v>
+        <v>0.88499999046325684</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
@@ -9418,21 +9418,21 @@
       </c>
       <c r="B5" s="1">
         <f>B1</f>
-        <v>1.3289999961853027</v>
+        <v>0.8880000114440918</v>
       </c>
       <c r="I5" s="2">
         <v>0</v>
       </c>
       <c r="J5" s="1">
         <f>B2</f>
-        <v>1.399399995803833</v>
+        <v>0.86239999532699585</v>
       </c>
       <c r="Q5" s="2">
         <v>0</v>
       </c>
       <c r="R5" s="1">
         <f>B3</f>
-        <v>1.3622000217437744</v>
+        <v>0.90740001201629639</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
@@ -9441,21 +9441,21 @@
       </c>
       <c r="B6" s="1">
         <f>C1</f>
-        <v>1.3059999942779541</v>
+        <v>0.8848000168800354</v>
       </c>
       <c r="I6" s="2">
         <v>3</v>
       </c>
       <c r="J6" s="1">
         <f>C2</f>
-        <v>1.3833999633789063</v>
+        <v>0.857200026512146</v>
       </c>
       <c r="Q6" s="2">
         <v>3</v>
       </c>
       <c r="R6" s="1">
         <f>C3</f>
-        <v>1.3263000249862671</v>
+        <v>0.89139997959136963</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -9464,21 +9464,21 @@
       </c>
       <c r="B7" s="1">
         <f>D1</f>
-        <v>1.2795000076293945</v>
+        <v>0.87720000743865967</v>
       </c>
       <c r="I7" s="2">
         <v>6</v>
       </c>
       <c r="J7" s="1">
         <f>D2</f>
-        <v>1.3614000082015991</v>
+        <v>0.84170001745223999</v>
       </c>
       <c r="Q7" s="2">
         <v>6</v>
       </c>
       <c r="R7" s="1">
         <f>D3</f>
-        <v>1.3035999536514282</v>
+        <v>0.88730001449584961</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
@@ -9487,21 +9487,21 @@
       </c>
       <c r="B8" s="1">
         <f>E1</f>
-        <v>1.2847000360488892</v>
+        <v>0.87529999017715454</v>
       </c>
       <c r="I8" s="2">
         <v>9</v>
       </c>
       <c r="J8" s="1">
         <f>E2</f>
-        <v>1.3514000177383423</v>
+        <v>0.84530001878738403</v>
       </c>
       <c r="Q8" s="2">
         <v>9</v>
       </c>
       <c r="R8" s="1">
         <f>E3</f>
-        <v>1.312999963760376</v>
+        <v>0.88489997386932373</v>
       </c>
       <c r="U8" s="8"/>
     </row>
@@ -9511,21 +9511,21 @@
       </c>
       <c r="B9" s="1">
         <f>F1</f>
-        <v>1.2824000120162964</v>
+        <v>0.87760001420974731</v>
       </c>
       <c r="I9" s="2">
         <v>12</v>
       </c>
       <c r="J9" s="1">
         <f>F2</f>
-        <v>1.3507000207901001</v>
+        <v>0.84049999713897705</v>
       </c>
       <c r="Q9" s="2">
         <v>12</v>
       </c>
       <c r="R9" s="1">
         <f>F3</f>
-        <v>1.3071000576019287</v>
+        <v>0.88510000705718994</v>
       </c>
       <c r="U9" s="8"/>
     </row>
@@ -9535,21 +9535,21 @@
       </c>
       <c r="B10" s="1">
         <f>G1</f>
-        <v>1.2856999635696411</v>
+        <v>0.87650001049041748</v>
       </c>
       <c r="I10" s="2">
         <v>15</v>
       </c>
       <c r="J10" s="1">
         <f>G2</f>
-        <v>1.351099967956543</v>
+        <v>0.83960002660751343</v>
       </c>
       <c r="Q10" s="2">
         <v>15</v>
       </c>
       <c r="R10" s="1">
         <f>G3</f>
-        <v>1.3101999759674072</v>
+        <v>0.88580000400543213</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
@@ -9558,21 +9558,21 @@
       </c>
       <c r="B11" s="1">
         <f>H1</f>
-        <v>1.2853000164031982</v>
+        <v>0.87589997053146362</v>
       </c>
       <c r="I11" s="2">
         <v>18</v>
       </c>
       <c r="J11" s="1">
         <f>H2</f>
-        <v>1.3523999452590942</v>
+        <v>0.83850002288818359</v>
       </c>
       <c r="Q11" s="2">
         <v>18</v>
       </c>
       <c r="R11" s="1">
         <f>H3</f>
-        <v>1.3055000305175781</v>
+        <v>0.88550001382827759</v>
       </c>
       <c r="U11" s="8"/>
     </row>
@@ -9582,21 +9582,21 @@
       </c>
       <c r="B12" s="1">
         <f>I1</f>
-        <v>1.2868000268936157</v>
+        <v>0.87459999322891235</v>
       </c>
       <c r="I12" s="2">
         <v>21</v>
       </c>
       <c r="J12" s="1">
         <f>I2</f>
-        <v>1.3540999889373779</v>
+        <v>0.83600002527236938</v>
       </c>
       <c r="Q12" s="2">
         <v>21</v>
       </c>
       <c r="R12" s="1">
         <f>I3</f>
-        <v>1.3092000484466553</v>
+        <v>0.88569998741149902</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
@@ -9605,21 +9605,21 @@
       </c>
       <c r="B13" s="1">
         <f>J1</f>
-        <v>1.2869999408721924</v>
+        <v>0.87319999933242798</v>
       </c>
       <c r="I13" s="2">
         <v>24</v>
       </c>
       <c r="J13" s="1">
         <f>J2</f>
-        <v>1.3549000024795532</v>
+        <v>0.83520001173019409</v>
       </c>
       <c r="Q13" s="2">
         <v>24</v>
       </c>
       <c r="R13" s="1">
         <f>J3</f>
-        <v>1.3027000427246094</v>
+        <v>0.88539999723434448</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
@@ -9628,21 +9628,21 @@
       </c>
       <c r="B14" s="1">
         <f>K1</f>
-        <v>1.2861000299453735</v>
+        <v>0.87339997291564941</v>
       </c>
       <c r="I14" s="2">
         <v>27</v>
       </c>
       <c r="J14" s="1">
         <f>K2</f>
-        <v>1.3532999753952026</v>
+        <v>0.83410000801086426</v>
       </c>
       <c r="Q14" s="2">
         <v>27</v>
       </c>
       <c r="R14" s="1">
         <f>K3</f>
-        <v>1.304900050163269</v>
+        <v>0.88529998064041138</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
@@ -9651,21 +9651,21 @@
       </c>
       <c r="B15" s="1">
         <f>L1</f>
-        <v>1.2847000360488892</v>
+        <v>0.87290000915527344</v>
       </c>
       <c r="I15" s="2">
         <v>30</v>
       </c>
       <c r="J15" s="1">
         <f>L2</f>
-        <v>1.3529000282287598</v>
+        <v>0.8345000147819519</v>
       </c>
       <c r="Q15" s="2">
         <v>30</v>
       </c>
       <c r="R15" s="1">
         <f>L3</f>
-        <v>1.305899977684021</v>
+        <v>0.88499999046325684</v>
       </c>
     </row>
   </sheetData>
@@ -9678,8 +9678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:O95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9701,44 +9701,44 @@
         <v>12</v>
       </c>
       <c r="B4" s="1">
-        <v>1.3969000577926636</v>
+        <v>0.74210000038146973</v>
       </c>
       <c r="C4" s="1">
-        <v>1.4208999872207642</v>
+        <v>0.75840002298355103</v>
       </c>
       <c r="D4" s="1">
-        <v>1.4388999938964844</v>
+        <v>0.77259999513626099</v>
       </c>
       <c r="E4" s="1">
-        <v>1.4895999431610107</v>
+        <v>0.7882000207901001</v>
       </c>
       <c r="F4" s="1">
-        <v>1.5183999538421631</v>
+        <v>0.79540002346038818</v>
       </c>
       <c r="G4" s="1">
-        <v>1.5471999645233154</v>
+        <v>0.81190001964569092</v>
       </c>
       <c r="H4" s="1">
-        <v>1.5745999813079834</v>
+        <v>0.82440000772476196</v>
       </c>
       <c r="I4" s="1">
-        <v>1.6004999876022339</v>
+        <v>0.8343999981880188</v>
       </c>
       <c r="J4" s="1">
-        <v>1.6236000061035156</v>
+        <v>0.84450000524520874</v>
       </c>
       <c r="K4" s="1">
-        <v>1.6440999507904053</v>
+        <v>0.85280001163482666</v>
       </c>
       <c r="L4" s="1">
-        <v>1.6655000448226929</v>
+        <v>0.86330002546310425</v>
       </c>
       <c r="N4" s="2">
         <v>0</v>
       </c>
       <c r="O4" s="2">
         <f>B6</f>
-        <v>1.3969000577926636</v>
+        <v>0.74210000038146973</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -9747,7 +9747,7 @@
       </c>
       <c r="O5" s="2">
         <f>C6</f>
-        <v>1.4208999872207642</v>
+        <v>0.75840002298355103</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -9756,54 +9756,54 @@
       </c>
       <c r="B6" s="2">
         <f>B4</f>
-        <v>1.3969000577926636</v>
+        <v>0.74210000038146973</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" ref="C6:L6" si="0">C4</f>
-        <v>1.4208999872207642</v>
+        <v>0.75840002298355103</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>1.4388999938964844</v>
+        <v>0.77259999513626099</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="0"/>
-        <v>1.4895999431610107</v>
+        <v>0.7882000207901001</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="0"/>
-        <v>1.5183999538421631</v>
+        <v>0.79540002346038818</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="0"/>
-        <v>1.5471999645233154</v>
+        <v>0.81190001964569092</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" si="0"/>
-        <v>1.5745999813079834</v>
+        <v>0.82440000772476196</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" si="0"/>
-        <v>1.6004999876022339</v>
+        <v>0.8343999981880188</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" si="0"/>
-        <v>1.6236000061035156</v>
+        <v>0.84450000524520874</v>
       </c>
       <c r="K6" s="2">
         <f t="shared" si="0"/>
-        <v>1.6440999507904053</v>
+        <v>0.85280001163482666</v>
       </c>
       <c r="L6" s="2">
         <f t="shared" si="0"/>
-        <v>1.6655000448226929</v>
+        <v>0.86330002546310425</v>
       </c>
       <c r="N6" s="2">
         <v>6</v>
       </c>
       <c r="O6" s="2">
         <f>D6</f>
-        <v>1.4388999938964844</v>
+        <v>0.77259999513626099</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -9812,7 +9812,7 @@
       </c>
       <c r="O7" s="2">
         <f>E6</f>
-        <v>1.4895999431610107</v>
+        <v>0.7882000207901001</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -9821,7 +9821,7 @@
       </c>
       <c r="O8" s="2">
         <f>F6</f>
-        <v>1.5183999538421631</v>
+        <v>0.79540002346038818</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -9830,7 +9830,7 @@
       </c>
       <c r="O9" s="2">
         <f>G6</f>
-        <v>1.5471999645233154</v>
+        <v>0.81190001964569092</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -9839,7 +9839,7 @@
       </c>
       <c r="O10" s="2">
         <f>H6</f>
-        <v>1.5745999813079834</v>
+        <v>0.82440000772476196</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -9848,7 +9848,7 @@
       </c>
       <c r="O11" s="2">
         <f>I6</f>
-        <v>1.6004999876022339</v>
+        <v>0.8343999981880188</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -9857,7 +9857,7 @@
       </c>
       <c r="O12" s="2">
         <f>J6</f>
-        <v>1.6236000061035156</v>
+        <v>0.84450000524520874</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -9866,7 +9866,7 @@
       </c>
       <c r="O13" s="2">
         <f>K6</f>
-        <v>1.6440999507904053</v>
+        <v>0.85280001163482666</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -9875,7 +9875,7 @@
       </c>
       <c r="O14" s="2">
         <f>L6</f>
-        <v>1.6655000448226929</v>
+        <v>0.86330002546310425</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -9886,44 +9886,44 @@
         <v>13</v>
       </c>
       <c r="B19" s="1">
-        <v>1.3562999963760376</v>
+        <v>0.82499998807907104</v>
       </c>
       <c r="C19" s="1">
-        <v>1.3845000267028809</v>
+        <v>0.82160001993179321</v>
       </c>
       <c r="D19" s="1">
-        <v>1.4154000282287598</v>
+        <v>0.80909997224807739</v>
       </c>
       <c r="E19" s="1">
-        <v>1.4664000272750854</v>
+        <v>0.8180999755859375</v>
       </c>
       <c r="F19" s="1">
-        <v>1.4980000257492065</v>
+        <v>0.83279997110366821</v>
       </c>
       <c r="G19" s="1">
-        <v>1.5290999412536621</v>
+        <v>0.83939999341964722</v>
       </c>
       <c r="H19" s="1">
-        <v>1.5597000122070313</v>
+        <v>0.8475000262260437</v>
       </c>
       <c r="I19" s="1">
-        <v>1.5860999822616577</v>
+        <v>0.86009997129440308</v>
       </c>
       <c r="J19" s="1">
-        <v>1.6126999855041504</v>
+        <v>0.87599998712539673</v>
       </c>
       <c r="K19" s="1">
-        <v>1.6338000297546387</v>
+        <v>0.88910001516342163</v>
       </c>
       <c r="L19" s="1">
-        <v>1.6562999486923218</v>
+        <v>0.90630000829696655</v>
       </c>
       <c r="N19" s="2">
         <v>0</v>
       </c>
       <c r="O19" s="2">
         <f>B21</f>
-        <v>1.3562999963760376</v>
+        <v>0.82499998807907104</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -9932,7 +9932,7 @@
       </c>
       <c r="O20" s="2">
         <f>C21</f>
-        <v>1.3845000267028809</v>
+        <v>0.82160001993179321</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -9941,54 +9941,54 @@
       </c>
       <c r="B21" s="2">
         <f>B19</f>
-        <v>1.3562999963760376</v>
+        <v>0.82499998807907104</v>
       </c>
       <c r="C21" s="2">
         <f t="shared" ref="C21:L21" si="1">C19</f>
-        <v>1.3845000267028809</v>
+        <v>0.82160001993179321</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="1"/>
-        <v>1.4154000282287598</v>
+        <v>0.80909997224807739</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" si="1"/>
-        <v>1.4664000272750854</v>
+        <v>0.8180999755859375</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="1"/>
-        <v>1.4980000257492065</v>
+        <v>0.83279997110366821</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" si="1"/>
-        <v>1.5290999412536621</v>
+        <v>0.83939999341964722</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" si="1"/>
-        <v>1.5597000122070313</v>
+        <v>0.8475000262260437</v>
       </c>
       <c r="I21" s="2">
         <f t="shared" si="1"/>
-        <v>1.5860999822616577</v>
+        <v>0.86009997129440308</v>
       </c>
       <c r="J21" s="2">
         <f t="shared" si="1"/>
-        <v>1.6126999855041504</v>
+        <v>0.87599998712539673</v>
       </c>
       <c r="K21" s="2">
         <f t="shared" si="1"/>
-        <v>1.6338000297546387</v>
+        <v>0.88910001516342163</v>
       </c>
       <c r="L21" s="2">
         <f t="shared" si="1"/>
-        <v>1.6562999486923218</v>
+        <v>0.90630000829696655</v>
       </c>
       <c r="N21" s="2">
         <v>6</v>
       </c>
       <c r="O21" s="2">
         <f>D21</f>
-        <v>1.4154000282287598</v>
+        <v>0.80909997224807739</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -9997,7 +9997,7 @@
       </c>
       <c r="O22" s="2">
         <f>E21</f>
-        <v>1.4664000272750854</v>
+        <v>0.8180999755859375</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -10006,7 +10006,7 @@
       </c>
       <c r="O23" s="2">
         <f>F21</f>
-        <v>1.4980000257492065</v>
+        <v>0.83279997110366821</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -10015,7 +10015,7 @@
       </c>
       <c r="O24" s="2">
         <f>G21</f>
-        <v>1.5290999412536621</v>
+        <v>0.83939999341964722</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -10024,7 +10024,7 @@
       </c>
       <c r="O25" s="2">
         <f>H21</f>
-        <v>1.5597000122070313</v>
+        <v>0.8475000262260437</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -10033,7 +10033,7 @@
       </c>
       <c r="O26" s="2">
         <f>I21</f>
-        <v>1.5860999822616577</v>
+        <v>0.86009997129440308</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -10042,7 +10042,7 @@
       </c>
       <c r="O27" s="2">
         <f>J21</f>
-        <v>1.6126999855041504</v>
+        <v>0.87599998712539673</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
@@ -10051,7 +10051,7 @@
       </c>
       <c r="O28" s="2">
         <f>K21</f>
-        <v>1.6338000297546387</v>
+        <v>0.88910001516342163</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -10060,7 +10060,7 @@
       </c>
       <c r="O29" s="2">
         <f>L21</f>
-        <v>1.6562999486923218</v>
+        <v>0.90630000829696655</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
@@ -10068,44 +10068,44 @@
         <v>14</v>
       </c>
       <c r="B35" s="1">
-        <v>1.4602999687194824</v>
+        <v>0.99059998989105225</v>
       </c>
       <c r="C35" s="1">
-        <v>1.4881000518798828</v>
+        <v>0.99639999866485596</v>
       </c>
       <c r="D35" s="1">
-        <v>1.5125000476837158</v>
+        <v>1.006100058555603</v>
       </c>
       <c r="E35" s="1">
-        <v>1.5582000017166138</v>
+        <v>1.0099999904632568</v>
       </c>
       <c r="F35" s="1">
-        <v>1.5859999656677246</v>
+        <v>1.0205999612808228</v>
       </c>
       <c r="G35" s="1">
-        <v>1.6171000003814697</v>
+        <v>1.0288000106811523</v>
       </c>
       <c r="H35" s="1">
-        <v>1.6435999870300293</v>
+        <v>1.0318000316619873</v>
       </c>
       <c r="I35" s="1">
-        <v>1.6694999933242798</v>
+        <v>1.0420999526977539</v>
       </c>
       <c r="J35" s="1">
-        <v>1.6948000192642212</v>
+        <v>1.0469000339508057</v>
       </c>
       <c r="K35" s="1">
-        <v>1.7158999443054199</v>
+        <v>1.0493999719619751</v>
       </c>
       <c r="L35" s="1">
-        <v>1.7395999431610107</v>
+        <v>1.0592999458312988</v>
       </c>
       <c r="N35" s="2">
         <v>0</v>
       </c>
       <c r="O35" s="2">
         <f>B37</f>
-        <v>1.4602999687194824</v>
+        <v>0.99059998989105225</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
@@ -10114,7 +10114,7 @@
       </c>
       <c r="O36" s="2">
         <f>C37</f>
-        <v>1.4881000518798828</v>
+        <v>0.99639999866485596</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
@@ -10123,54 +10123,54 @@
       </c>
       <c r="B37" s="2">
         <f>B35</f>
-        <v>1.4602999687194824</v>
+        <v>0.99059998989105225</v>
       </c>
       <c r="C37" s="2">
         <f t="shared" ref="C37:L37" si="2">C35</f>
-        <v>1.4881000518798828</v>
+        <v>0.99639999866485596</v>
       </c>
       <c r="D37" s="2">
         <f t="shared" si="2"/>
-        <v>1.5125000476837158</v>
+        <v>1.006100058555603</v>
       </c>
       <c r="E37" s="2">
         <f t="shared" si="2"/>
-        <v>1.5582000017166138</v>
+        <v>1.0099999904632568</v>
       </c>
       <c r="F37" s="2">
         <f t="shared" si="2"/>
-        <v>1.5859999656677246</v>
+        <v>1.0205999612808228</v>
       </c>
       <c r="G37" s="2">
         <f t="shared" si="2"/>
-        <v>1.6171000003814697</v>
+        <v>1.0288000106811523</v>
       </c>
       <c r="H37" s="2">
         <f t="shared" si="2"/>
-        <v>1.6435999870300293</v>
+        <v>1.0318000316619873</v>
       </c>
       <c r="I37" s="2">
         <f t="shared" si="2"/>
-        <v>1.6694999933242798</v>
+        <v>1.0420999526977539</v>
       </c>
       <c r="J37" s="2">
         <f t="shared" si="2"/>
-        <v>1.6948000192642212</v>
+        <v>1.0469000339508057</v>
       </c>
       <c r="K37" s="2">
         <f t="shared" si="2"/>
-        <v>1.7158999443054199</v>
+        <v>1.0493999719619751</v>
       </c>
       <c r="L37" s="2">
         <f t="shared" si="2"/>
-        <v>1.7395999431610107</v>
+        <v>1.0592999458312988</v>
       </c>
       <c r="N37" s="2">
         <v>6</v>
       </c>
       <c r="O37" s="2">
         <f>D37</f>
-        <v>1.5125000476837158</v>
+        <v>1.006100058555603</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
@@ -10179,7 +10179,7 @@
       </c>
       <c r="O38" s="2">
         <f>E37</f>
-        <v>1.5582000017166138</v>
+        <v>1.0099999904632568</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
@@ -10188,7 +10188,7 @@
       </c>
       <c r="O39" s="2">
         <f>F37</f>
-        <v>1.5859999656677246</v>
+        <v>1.0205999612808228</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
@@ -10197,7 +10197,7 @@
       </c>
       <c r="O40" s="2">
         <f>G37</f>
-        <v>1.6171000003814697</v>
+        <v>1.0288000106811523</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
@@ -10206,7 +10206,7 @@
       </c>
       <c r="O41" s="2">
         <f>H37</f>
-        <v>1.6435999870300293</v>
+        <v>1.0318000316619873</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.3">
@@ -10215,7 +10215,7 @@
       </c>
       <c r="O42" s="2">
         <f>I37</f>
-        <v>1.6694999933242798</v>
+        <v>1.0420999526977539</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
@@ -10225,7 +10225,7 @@
       </c>
       <c r="O43" s="2">
         <f>J37</f>
-        <v>1.6948000192642212</v>
+        <v>1.0469000339508057</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
@@ -10234,7 +10234,7 @@
       </c>
       <c r="O44" s="2">
         <f>K37</f>
-        <v>1.7158999443054199</v>
+        <v>1.0493999719619751</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
@@ -10243,7 +10243,7 @@
       </c>
       <c r="O45" s="2">
         <f>L37</f>
-        <v>1.7395999431610107</v>
+        <v>1.0592999458312988</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
@@ -10251,44 +10251,44 @@
         <v>15</v>
       </c>
       <c r="B51" s="1">
-        <v>1.468999981880188</v>
+        <v>0.8726000189781189</v>
       </c>
       <c r="C51" s="1">
-        <v>1.5075000524520874</v>
+        <v>0.89840000867843628</v>
       </c>
       <c r="D51" s="1">
-        <v>1.5296000242233276</v>
+        <v>0.90429997444152832</v>
       </c>
       <c r="E51" s="1">
-        <v>1.5700000524520874</v>
+        <v>0.91540002822875977</v>
       </c>
       <c r="F51" s="1">
-        <v>1.5918999910354614</v>
+        <v>0.92510002851486206</v>
       </c>
       <c r="G51" s="1">
-        <v>1.6202000379562378</v>
+        <v>0.93819999694824219</v>
       </c>
       <c r="H51" s="1">
-        <v>1.6440999507904053</v>
+        <v>0.94849997758865356</v>
       </c>
       <c r="I51" s="1">
-        <v>1.6651999950408936</v>
+        <v>0.96079999208450317</v>
       </c>
       <c r="J51" s="1">
-        <v>1.687999963760376</v>
+        <v>0.97310000658035278</v>
       </c>
       <c r="K51" s="1">
-        <v>1.7039999961853027</v>
+        <v>0.98290002346038818</v>
       </c>
       <c r="L51" s="1">
-        <v>1.7206000089645386</v>
+        <v>0.99459999799728394</v>
       </c>
       <c r="N51" s="2">
         <v>0</v>
       </c>
       <c r="O51" s="2">
         <f>B53</f>
-        <v>1.468999981880188</v>
+        <v>0.8726000189781189</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.3">
@@ -10297,7 +10297,7 @@
       </c>
       <c r="O52" s="2">
         <f>C53</f>
-        <v>1.5075000524520874</v>
+        <v>0.89840000867843628</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
@@ -10306,54 +10306,54 @@
       </c>
       <c r="B53" s="2">
         <f>B51</f>
-        <v>1.468999981880188</v>
+        <v>0.8726000189781189</v>
       </c>
       <c r="C53" s="2">
         <f t="shared" ref="C53:L53" si="3">C51</f>
-        <v>1.5075000524520874</v>
+        <v>0.89840000867843628</v>
       </c>
       <c r="D53" s="2">
         <f t="shared" si="3"/>
-        <v>1.5296000242233276</v>
+        <v>0.90429997444152832</v>
       </c>
       <c r="E53" s="2">
         <f t="shared" si="3"/>
-        <v>1.5700000524520874</v>
+        <v>0.91540002822875977</v>
       </c>
       <c r="F53" s="2">
         <f t="shared" si="3"/>
-        <v>1.5918999910354614</v>
+        <v>0.92510002851486206</v>
       </c>
       <c r="G53" s="2">
         <f t="shared" si="3"/>
-        <v>1.6202000379562378</v>
+        <v>0.93819999694824219</v>
       </c>
       <c r="H53" s="2">
         <f t="shared" si="3"/>
-        <v>1.6440999507904053</v>
+        <v>0.94849997758865356</v>
       </c>
       <c r="I53" s="2">
         <f t="shared" si="3"/>
-        <v>1.6651999950408936</v>
+        <v>0.96079999208450317</v>
       </c>
       <c r="J53" s="2">
         <f t="shared" si="3"/>
-        <v>1.687999963760376</v>
+        <v>0.97310000658035278</v>
       </c>
       <c r="K53" s="2">
         <f t="shared" si="3"/>
-        <v>1.7039999961853027</v>
+        <v>0.98290002346038818</v>
       </c>
       <c r="L53" s="2">
         <f t="shared" si="3"/>
-        <v>1.7206000089645386</v>
+        <v>0.99459999799728394</v>
       </c>
       <c r="N53" s="2">
         <v>6</v>
       </c>
       <c r="O53" s="2">
         <f>D53</f>
-        <v>1.5296000242233276</v>
+        <v>0.90429997444152832</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.3">
@@ -10362,7 +10362,7 @@
       </c>
       <c r="O54" s="2">
         <f>E53</f>
-        <v>1.5700000524520874</v>
+        <v>0.91540002822875977</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
@@ -10371,7 +10371,7 @@
       </c>
       <c r="O55" s="2">
         <f>F53</f>
-        <v>1.5918999910354614</v>
+        <v>0.92510002851486206</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.3">
@@ -10380,7 +10380,7 @@
       </c>
       <c r="O56" s="2">
         <f>G53</f>
-        <v>1.6202000379562378</v>
+        <v>0.93819999694824219</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
@@ -10389,7 +10389,7 @@
       </c>
       <c r="O57" s="2">
         <f>H53</f>
-        <v>1.6440999507904053</v>
+        <v>0.94849997758865356</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
@@ -10398,7 +10398,7 @@
       </c>
       <c r="O58" s="2">
         <f>I53</f>
-        <v>1.6651999950408936</v>
+        <v>0.96079999208450317</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
@@ -10407,7 +10407,7 @@
       </c>
       <c r="O59" s="2">
         <f>J53</f>
-        <v>1.687999963760376</v>
+        <v>0.97310000658035278</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.3">
@@ -10416,7 +10416,7 @@
       </c>
       <c r="O60" s="2">
         <f>K53</f>
-        <v>1.7039999961853027</v>
+        <v>0.98290002346038818</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.3">
@@ -10425,7 +10425,7 @@
       </c>
       <c r="O61" s="2">
         <f>L53</f>
-        <v>1.7206000089645386</v>
+        <v>0.99459999799728394</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.3">
@@ -10433,44 +10433,44 @@
         <v>16</v>
       </c>
       <c r="B68" s="1">
-        <v>1.4392999410629272</v>
+        <v>0.79860001802444458</v>
       </c>
       <c r="C68" s="1">
-        <v>1.4795000553131104</v>
+        <v>0.80739998817443848</v>
       </c>
       <c r="D68" s="1">
-        <v>1.5166000127792358</v>
+        <v>0.81650000810623169</v>
       </c>
       <c r="E68" s="1">
-        <v>1.5621999502182007</v>
+        <v>0.82719999551773071</v>
       </c>
       <c r="F68" s="1">
-        <v>1.5843000411987305</v>
+        <v>0.83890002965927124</v>
       </c>
       <c r="G68" s="1">
-        <v>1.6066000461578369</v>
+        <v>0.84939998388290405</v>
       </c>
       <c r="H68" s="1">
-        <v>1.6277999877929687</v>
+        <v>0.86009997129440308</v>
       </c>
       <c r="I68" s="1">
-        <v>1.6492999792098999</v>
+        <v>0.87070000171661377</v>
       </c>
       <c r="J68" s="1">
-        <v>1.6711000204086304</v>
+        <v>0.88129997253417969</v>
       </c>
       <c r="K68" s="1">
-        <v>1.6893999576568604</v>
+        <v>0.89179998636245728</v>
       </c>
       <c r="L68" s="1">
-        <v>1.7085000276565552</v>
+        <v>0.90179997682571411</v>
       </c>
       <c r="N68" s="2">
         <v>0</v>
       </c>
       <c r="O68" s="2">
         <f>B70</f>
-        <v>1.4392999410629272</v>
+        <v>0.79860001802444458</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.3">
@@ -10479,7 +10479,7 @@
       </c>
       <c r="O69" s="2">
         <f>C70</f>
-        <v>1.4795000553131104</v>
+        <v>0.80739998817443848</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.3">
@@ -10488,54 +10488,54 @@
       </c>
       <c r="B70" s="2">
         <f>B68</f>
-        <v>1.4392999410629272</v>
+        <v>0.79860001802444458</v>
       </c>
       <c r="C70" s="2">
         <f t="shared" ref="C70:L70" si="4">C68</f>
-        <v>1.4795000553131104</v>
+        <v>0.80739998817443848</v>
       </c>
       <c r="D70" s="2">
         <f t="shared" si="4"/>
-        <v>1.5166000127792358</v>
+        <v>0.81650000810623169</v>
       </c>
       <c r="E70" s="2">
         <f t="shared" si="4"/>
-        <v>1.5621999502182007</v>
+        <v>0.82719999551773071</v>
       </c>
       <c r="F70" s="2">
         <f t="shared" si="4"/>
-        <v>1.5843000411987305</v>
+        <v>0.83890002965927124</v>
       </c>
       <c r="G70" s="2">
         <f t="shared" si="4"/>
-        <v>1.6066000461578369</v>
+        <v>0.84939998388290405</v>
       </c>
       <c r="H70" s="2">
         <f t="shared" si="4"/>
-        <v>1.6277999877929687</v>
+        <v>0.86009997129440308</v>
       </c>
       <c r="I70" s="2">
         <f t="shared" si="4"/>
-        <v>1.6492999792098999</v>
+        <v>0.87070000171661377</v>
       </c>
       <c r="J70" s="2">
         <f t="shared" si="4"/>
-        <v>1.6711000204086304</v>
+        <v>0.88129997253417969</v>
       </c>
       <c r="K70" s="2">
         <f t="shared" si="4"/>
-        <v>1.6893999576568604</v>
+        <v>0.89179998636245728</v>
       </c>
       <c r="L70" s="2">
         <f t="shared" si="4"/>
-        <v>1.7085000276565552</v>
+        <v>0.90179997682571411</v>
       </c>
       <c r="N70" s="2">
         <v>6</v>
       </c>
       <c r="O70" s="2">
         <f>D70</f>
-        <v>1.5166000127792358</v>
+        <v>0.81650000810623169</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.3">
@@ -10544,7 +10544,7 @@
       </c>
       <c r="O71" s="2">
         <f>E70</f>
-        <v>1.5621999502182007</v>
+        <v>0.82719999551773071</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.3">
@@ -10553,7 +10553,7 @@
       </c>
       <c r="O72" s="2">
         <f>F70</f>
-        <v>1.5843000411987305</v>
+        <v>0.83890002965927124</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.3">
@@ -10562,7 +10562,7 @@
       </c>
       <c r="O73" s="2">
         <f>G70</f>
-        <v>1.6066000461578369</v>
+        <v>0.84939998388290405</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.3">
@@ -10571,7 +10571,7 @@
       </c>
       <c r="O74" s="2">
         <f>H70</f>
-        <v>1.6277999877929687</v>
+        <v>0.86009997129440308</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.3">
@@ -10580,7 +10580,7 @@
       </c>
       <c r="O75" s="2">
         <f>I70</f>
-        <v>1.6492999792098999</v>
+        <v>0.87070000171661377</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.3">
@@ -10589,7 +10589,7 @@
       </c>
       <c r="O76" s="2">
         <f>J70</f>
-        <v>1.6711000204086304</v>
+        <v>0.88129997253417969</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.3">
@@ -10598,7 +10598,7 @@
       </c>
       <c r="O77" s="2">
         <f>K70</f>
-        <v>1.6893999576568604</v>
+        <v>0.89179998636245728</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.3">
@@ -10607,7 +10607,7 @@
       </c>
       <c r="O78" s="2">
         <f>L70</f>
-        <v>1.7085000276565552</v>
+        <v>0.90179997682571411</v>
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.3">
@@ -10615,44 +10615,44 @@
         <v>17</v>
       </c>
       <c r="B85" s="1">
-        <v>1.4384000301361084</v>
+        <v>0.86070001125335693</v>
       </c>
       <c r="C85" s="1">
-        <v>1.4737000465393066</v>
+        <v>0.8694000244140625</v>
       </c>
       <c r="D85" s="1">
-        <v>1.4991999864578247</v>
+        <v>0.87449997663497925</v>
       </c>
       <c r="E85" s="1">
-        <v>1.5490000247955322</v>
+        <v>0.88440001010894775</v>
       </c>
       <c r="F85" s="1">
-        <v>1.5776000022888184</v>
+        <v>0.90039998292922974</v>
       </c>
       <c r="G85" s="1">
-        <v>1.6019999980926514</v>
+        <v>0.91720002889633179</v>
       </c>
       <c r="H85" s="1">
-        <v>1.6211999654769897</v>
+        <v>0.93580001592636108</v>
       </c>
       <c r="I85" s="1">
-        <v>1.638200044631958</v>
+        <v>0.95469999313354492</v>
       </c>
       <c r="J85" s="1">
-        <v>1.6539000272750854</v>
+        <v>0.9725000262260437</v>
       </c>
       <c r="K85" s="1">
-        <v>1.6684000492095947</v>
+        <v>0.99029999971389771</v>
       </c>
       <c r="L85" s="1">
-        <v>1.68340003490448</v>
+        <v>1.0054999589920044</v>
       </c>
       <c r="N85" s="2">
         <v>0</v>
       </c>
       <c r="O85" s="2">
         <f>B87</f>
-        <v>1.4384000301361084</v>
+        <v>0.86070001125335693</v>
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.3">
@@ -10661,7 +10661,7 @@
       </c>
       <c r="O86" s="2">
         <f>C87</f>
-        <v>1.4737000465393066</v>
+        <v>0.8694000244140625</v>
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.3">
@@ -10670,54 +10670,54 @@
       </c>
       <c r="B87" s="2">
         <f>B85</f>
-        <v>1.4384000301361084</v>
+        <v>0.86070001125335693</v>
       </c>
       <c r="C87" s="2">
         <f t="shared" ref="C87:L87" si="5">C85</f>
-        <v>1.4737000465393066</v>
+        <v>0.8694000244140625</v>
       </c>
       <c r="D87" s="2">
         <f t="shared" si="5"/>
-        <v>1.4991999864578247</v>
+        <v>0.87449997663497925</v>
       </c>
       <c r="E87" s="2">
         <f t="shared" si="5"/>
-        <v>1.5490000247955322</v>
+        <v>0.88440001010894775</v>
       </c>
       <c r="F87" s="2">
         <f t="shared" si="5"/>
-        <v>1.5776000022888184</v>
+        <v>0.90039998292922974</v>
       </c>
       <c r="G87" s="2">
         <f t="shared" si="5"/>
-        <v>1.6019999980926514</v>
+        <v>0.91720002889633179</v>
       </c>
       <c r="H87" s="2">
         <f t="shared" si="5"/>
-        <v>1.6211999654769897</v>
+        <v>0.93580001592636108</v>
       </c>
       <c r="I87" s="2">
         <f t="shared" si="5"/>
-        <v>1.638200044631958</v>
+        <v>0.95469999313354492</v>
       </c>
       <c r="J87" s="2">
         <f t="shared" si="5"/>
-        <v>1.6539000272750854</v>
+        <v>0.9725000262260437</v>
       </c>
       <c r="K87" s="2">
         <f t="shared" si="5"/>
-        <v>1.6684000492095947</v>
+        <v>0.99029999971389771</v>
       </c>
       <c r="L87" s="2">
         <f t="shared" si="5"/>
-        <v>1.68340003490448</v>
+        <v>1.0054999589920044</v>
       </c>
       <c r="N87" s="2">
         <v>6</v>
       </c>
       <c r="O87" s="2">
         <f>D87</f>
-        <v>1.4991999864578247</v>
+        <v>0.87449997663497925</v>
       </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.3">
@@ -10726,7 +10726,7 @@
       </c>
       <c r="O88" s="2">
         <f>E87</f>
-        <v>1.5490000247955322</v>
+        <v>0.88440001010894775</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.3">
@@ -10735,7 +10735,7 @@
       </c>
       <c r="O89" s="2">
         <f>F87</f>
-        <v>1.5776000022888184</v>
+        <v>0.90039998292922974</v>
       </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.3">
@@ -10744,7 +10744,7 @@
       </c>
       <c r="O90" s="2">
         <f>G87</f>
-        <v>1.6019999980926514</v>
+        <v>0.91720002889633179</v>
       </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.3">
@@ -10753,7 +10753,7 @@
       </c>
       <c r="O91" s="2">
         <f>H87</f>
-        <v>1.6211999654769897</v>
+        <v>0.93580001592636108</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.3">
@@ -10762,7 +10762,7 @@
       </c>
       <c r="O92" s="2">
         <f>I87</f>
-        <v>1.638200044631958</v>
+        <v>0.95469999313354492</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.3">
@@ -10771,7 +10771,7 @@
       </c>
       <c r="O93" s="2">
         <f>J87</f>
-        <v>1.6539000272750854</v>
+        <v>0.9725000262260437</v>
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.3">
@@ -10780,7 +10780,7 @@
       </c>
       <c r="O94" s="2">
         <f>K87</f>
-        <v>1.6684000492095947</v>
+        <v>0.99029999971389771</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.3">
@@ -10789,7 +10789,7 @@
       </c>
       <c r="O95" s="2">
         <f>L87</f>
-        <v>1.68340003490448</v>
+        <v>1.0054999589920044</v>
       </c>
     </row>
   </sheetData>
@@ -10804,7 +10804,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10856,7 +10856,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
-        <v>91213</v>
+        <v>91214</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>21</v>
@@ -10865,28 +10865,28 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>9.2999999999999992E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="E3" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" ref="F3:F8" si="0">D3-E3</f>
-        <v>9.0999999999999987E-3</v>
+        <v>3.8E-3</v>
       </c>
       <c r="G3" s="1">
-        <v>6.25E-2</v>
+        <v>6.6100000000000006E-2</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H8" si="1">F3/G3</f>
-        <v>0.14559999999999998</v>
+        <v>5.7488653555219357E-2</v>
       </c>
       <c r="I3" s="6">
-        <v>74.234354194407445</v>
+        <v>77.86666666666666</v>
       </c>
       <c r="J3" s="6">
         <f t="shared" ref="J3:J8" si="2">(H3*60*50000*100)/(1000*50*0.6*I3)</f>
-        <v>19.613560538116591</v>
+        <v>7.3829606449339913</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -10896,28 +10896,28 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>1.03E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="E4" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>1.01E-2</v>
+        <v>2.8E-3</v>
       </c>
       <c r="G4" s="1">
-        <v>6.25E-2</v>
+        <v>6.6100000000000006E-2</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="1"/>
-        <v>0.16159999999999999</v>
+        <v>4.2360060514372161E-2</v>
       </c>
       <c r="I4" s="6">
-        <v>74.234354194407445</v>
+        <v>77.86666666666666</v>
       </c>
       <c r="J4" s="6">
         <f t="shared" si="2"/>
-        <v>21.768896860986551</v>
+        <v>5.4400762646882059</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -10927,28 +10927,28 @@
         <v>3</v>
       </c>
       <c r="D5">
-        <v>9.4999999999999998E-3</v>
+        <v>2.3E-3</v>
       </c>
       <c r="E5" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>9.2999999999999992E-3</v>
+        <v>2.0999999999999999E-3</v>
       </c>
       <c r="G5" s="1">
-        <v>6.25E-2</v>
+        <v>6.6100000000000006E-2</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="1"/>
-        <v>0.14879999999999999</v>
+        <v>3.1770045385779121E-2</v>
       </c>
       <c r="I5" s="6">
-        <v>74.234354194407445</v>
+        <v>77.86666666666666</v>
       </c>
       <c r="J5" s="6">
         <f t="shared" si="2"/>
-        <v>20.044627802690584</v>
+        <v>4.0800571985161547</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -10958,28 +10958,28 @@
         <v>4</v>
       </c>
       <c r="D6">
-        <v>8.3999999999999995E-3</v>
+        <v>3.8E-3</v>
       </c>
       <c r="E6" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>8.199999999999999E-3</v>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="G6" s="1">
-        <v>6.25E-2</v>
+        <v>6.6100000000000006E-2</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
-        <v>0.13119999999999998</v>
+        <v>5.4462934947049915E-2</v>
       </c>
       <c r="I6" s="6">
-        <v>74.234354194407445</v>
+        <v>77.86666666666666</v>
       </c>
       <c r="J6" s="6">
         <f t="shared" si="2"/>
-        <v>17.673757847533633</v>
+        <v>6.9943837688848349</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -10989,28 +10989,28 @@
         <v>5</v>
       </c>
       <c r="D7">
-        <v>8.6999999999999994E-3</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="E7" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>8.4999999999999989E-3</v>
+        <v>3.3E-3</v>
       </c>
       <c r="G7" s="1">
-        <v>6.25E-2</v>
+        <v>6.6100000000000006E-2</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="1"/>
-        <v>0.13599999999999998</v>
+        <v>4.9924357034795759E-2</v>
       </c>
       <c r="I7" s="6">
-        <v>74.234354194407445</v>
+        <v>77.86666666666666</v>
       </c>
       <c r="J7" s="6">
         <f t="shared" si="2"/>
-        <v>18.320358744394618</v>
+        <v>6.4115184548110982</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -11020,28 +11020,28 @@
         <v>6</v>
       </c>
       <c r="D8">
-        <v>8.2000000000000007E-3</v>
+        <v>5.1000000000000004E-3</v>
       </c>
       <c r="E8" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="0"/>
-        <v>8.0000000000000002E-3</v>
+        <v>4.9000000000000007E-3</v>
       </c>
       <c r="G8" s="1">
-        <v>6.25E-2</v>
+        <v>6.6100000000000006E-2</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="1"/>
-        <v>0.128</v>
+        <v>7.4130105900151289E-2</v>
       </c>
       <c r="I8" s="6">
-        <v>74.234354194407445</v>
+        <v>77.86666666666666</v>
       </c>
       <c r="J8" s="6">
         <f t="shared" si="2"/>
-        <v>17.242690582959643</v>
+        <v>9.5201334632043597</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>